<commit_message>
Initial commit with project structure and gitignore
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Desktop\Final Project\TripPlanner\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Desktop\TripPlanner_Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336CBD78-CD50-4D73-80FD-35AF6FF5282E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B63F99-3D16-4557-B50C-9CC4E726883F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2664" yWindow="3228" windowWidth="17280" windowHeight="8880" xr2:uid="{ED7731E5-9524-457D-ACFC-E87F166DBFF7}"/>
+    <workbookView xWindow="2664" yWindow="3228" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{ED7731E5-9524-457D-ACFC-E87F166DBFF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="3" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>TripAdvisorURL</t>
   </si>
   <si>
-    <t>https://www.tripadvisor.com</t>
-  </si>
-  <si>
     <t>Target application URL</t>
   </si>
   <si>
@@ -92,16 +89,27 @@
   </si>
   <si>
     <t>Asset</t>
+  </si>
+  <si>
+    <t>https://www.getyourguide.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,13 +132,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FDBBE9-D6D9-4DCB-B2CC-5A2F9C80B171}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -481,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -513,24 +524,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -542,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673D08A6-97E6-40BE-8CEC-276A9D3C9FCC}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,36 +579,39 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9933614C-7841-4987-9FB7-F7F945AD3CF1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>